<commit_message>
Added Delete customer test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Problem solving with Rohit\APIautomation\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11036E7F-817A-4B53-85A6-0A83D7615023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5284D96-B887-43D7-9D5C-F12BD713D350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -36,9 +36,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>alak</t>
   </si>
   <si>
@@ -66,7 +63,22 @@
     <t>r@gmail.com</t>
   </si>
   <si>
-    <t>this is the first test</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>deleteCustomer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>This is the first test</t>
+  </si>
+  <si>
+    <t>This is the second test</t>
+  </si>
+  <si>
+    <t>This is the third test</t>
   </si>
 </sst>
 </file>
@@ -404,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,7 +430,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -434,40 +446,40 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -483,13 +495,28 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Utilities and Deleted Customer test case are added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Problem solving with Rohit\APIautomation\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5284D96-B887-43D7-9D5C-F12BD713D350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF5D982-1340-47E1-8F90-27964D3385B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>This is the third test</t>
+  </si>
+  <si>
+    <t>cus_IBc0ERhRyxXWsL</t>
+  </si>
+  <si>
+    <t>cus_IBc00mEJZdW8Kg</t>
+  </si>
+  <si>
+    <t>cus_IBc09g64O3FaQE</t>
+  </si>
+  <si>
+    <t>cus_IBc0ej42CA1Txb</t>
+  </si>
+  <si>
+    <t>cus_IBc0J46XloVal7</t>
+  </si>
+  <si>
+    <t>cus_IBc0swmV0KXVgB</t>
   </si>
 </sst>
 </file>
@@ -419,7 +437,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,7 +532,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>14</v>
       </c>

</xml_diff>